<commit_message>
created a workflow to test from an excel file. the file can be filled using a shiny app. added enabler mv 3 functionality
</commit_message>
<xml_diff>
--- a/inst/extdata/decklist.xlsx
+++ b/inst/extdata/decklist.xlsx
@@ -81,9 +81,6 @@
     <t>Commandeer</t>
   </si>
   <si>
-    <t>Consign</t>
-  </si>
-  <si>
     <t>Contagion</t>
   </si>
   <si>
@@ -120,9 +117,6 @@
     <t>Fallen Shinobi</t>
   </si>
   <si>
-    <t>Far</t>
-  </si>
-  <si>
     <t>Fierce Guardianship</t>
   </si>
   <si>
@@ -418,6 +412,12 @@
   </si>
   <si>
     <t>card_name</t>
+  </si>
+  <si>
+    <t>ConsignOblivion</t>
+  </si>
+  <si>
+    <t>FarAway</t>
   </si>
 </sst>
 </file>
@@ -761,7 +761,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomLeft" activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,76 +775,76 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" t="s">
         <v>117</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" t="s">
         <v>99</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
+        <v>119</v>
+      </c>
+      <c r="K1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L1" t="s">
         <v>100</v>
       </c>
-      <c r="F1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G1" t="s">
-        <v>118</v>
-      </c>
-      <c r="H1" t="s">
-        <v>120</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
+        <v>121</v>
+      </c>
+      <c r="N1" t="s">
+        <v>122</v>
+      </c>
+      <c r="O1" t="s">
+        <v>103</v>
+      </c>
+      <c r="P1" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="R1" t="s">
         <v>101</v>
       </c>
-      <c r="J1" t="s">
-        <v>121</v>
-      </c>
-      <c r="K1" t="s">
-        <v>122</v>
-      </c>
-      <c r="L1" t="s">
-        <v>102</v>
-      </c>
-      <c r="M1" t="s">
-        <v>123</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="S1" t="s">
         <v>124</v>
       </c>
-      <c r="O1" t="s">
-        <v>105</v>
-      </c>
-      <c r="P1" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="R1" t="s">
-        <v>103</v>
-      </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
+        <v>125</v>
+      </c>
+      <c r="U1" t="s">
         <v>126</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>127</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>128</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>129</v>
-      </c>
-      <c r="W1" t="s">
-        <v>130</v>
-      </c>
-      <c r="X1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
@@ -1589,7 +1589,7 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>131</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1663,7 +1663,7 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1737,7 +1737,7 @@
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1811,7 +1811,7 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1885,7 +1885,7 @@
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1959,7 +1959,7 @@
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2033,7 +2033,7 @@
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -2107,7 +2107,7 @@
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -2181,7 +2181,7 @@
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -2255,7 +2255,7 @@
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -2329,7 +2329,7 @@
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -2403,7 +2403,7 @@
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -2477,7 +2477,7 @@
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -2551,7 +2551,7 @@
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>132</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -2625,7 +2625,7 @@
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -2699,7 +2699,7 @@
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -2773,7 +2773,7 @@
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -2847,7 +2847,7 @@
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -2921,7 +2921,7 @@
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -2995,7 +2995,7 @@
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -3069,7 +3069,7 @@
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -3143,7 +3143,7 @@
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -3217,7 +3217,7 @@
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -3291,7 +3291,7 @@
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -3318,10 +3318,10 @@
         <v>1</v>
       </c>
       <c r="J35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L35">
         <v>0</v>
@@ -3365,7 +3365,7 @@
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -3439,7 +3439,7 @@
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -3513,7 +3513,7 @@
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -3587,7 +3587,7 @@
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -3661,7 +3661,7 @@
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -3735,7 +3735,7 @@
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -3809,7 +3809,7 @@
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -3883,7 +3883,7 @@
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -3957,7 +3957,7 @@
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -4031,7 +4031,7 @@
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -4105,7 +4105,7 @@
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -4179,7 +4179,7 @@
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -4253,7 +4253,7 @@
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -4327,7 +4327,7 @@
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -4401,7 +4401,7 @@
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -4475,7 +4475,7 @@
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -4549,7 +4549,7 @@
     </row>
     <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -4623,7 +4623,7 @@
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -4697,7 +4697,7 @@
     </row>
     <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -4771,7 +4771,7 @@
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -4845,7 +4845,7 @@
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -4919,7 +4919,7 @@
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B57">
         <v>1</v>
@@ -4993,7 +4993,7 @@
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -5067,7 +5067,7 @@
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -5141,7 +5141,7 @@
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -5215,7 +5215,7 @@
     </row>
     <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -5289,7 +5289,7 @@
     </row>
     <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B62">
         <v>1</v>
@@ -5363,7 +5363,7 @@
     </row>
     <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B63">
         <v>1</v>
@@ -5437,7 +5437,7 @@
     </row>
     <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -5511,7 +5511,7 @@
     </row>
     <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -5585,7 +5585,7 @@
     </row>
     <row r="66" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -5659,7 +5659,7 @@
     </row>
     <row r="67" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -5733,7 +5733,7 @@
     </row>
     <row r="68" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B68">
         <v>1</v>
@@ -5807,7 +5807,7 @@
     </row>
     <row r="69" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -5881,7 +5881,7 @@
     </row>
     <row r="70" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B70">
         <v>1</v>
@@ -5955,7 +5955,7 @@
     </row>
     <row r="71" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B71">
         <v>1</v>
@@ -6029,7 +6029,7 @@
     </row>
     <row r="72" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -6103,7 +6103,7 @@
     </row>
     <row r="73" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B73">
         <v>1</v>
@@ -6177,7 +6177,7 @@
     </row>
     <row r="74" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -6251,7 +6251,7 @@
     </row>
     <row r="75" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B75">
         <v>1</v>
@@ -6325,7 +6325,7 @@
     </row>
     <row r="76" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B76">
         <v>1</v>
@@ -6399,7 +6399,7 @@
     </row>
     <row r="77" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B77">
         <v>1</v>
@@ -6473,7 +6473,7 @@
     </row>
     <row r="78" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B78">
         <v>1</v>
@@ -6547,7 +6547,7 @@
     </row>
     <row r="79" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B79">
         <v>1</v>
@@ -6621,7 +6621,7 @@
     </row>
     <row r="80" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B80">
         <v>1</v>
@@ -6695,7 +6695,7 @@
     </row>
     <row r="81" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B81">
         <v>1</v>
@@ -6769,7 +6769,7 @@
     </row>
     <row r="82" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B82">
         <v>1</v>
@@ -6843,7 +6843,7 @@
     </row>
     <row r="83" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B83">
         <v>1</v>
@@ -6917,7 +6917,7 @@
     </row>
     <row r="84" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -6991,7 +6991,7 @@
     </row>
     <row r="85" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -7065,7 +7065,7 @@
     </row>
     <row r="86" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B86">
         <v>1</v>
@@ -7139,7 +7139,7 @@
     </row>
     <row r="87" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B87">
         <v>1</v>
@@ -7213,7 +7213,7 @@
     </row>
     <row r="88" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -7287,7 +7287,7 @@
     </row>
     <row r="89" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B89">
         <v>1</v>
@@ -7361,7 +7361,7 @@
     </row>
     <row r="90" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B90">
         <v>1</v>
@@ -7435,7 +7435,7 @@
     </row>
     <row r="91" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B91">
         <v>1</v>
@@ -7509,7 +7509,7 @@
     </row>
     <row r="92" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B92">
         <v>1</v>
@@ -7583,7 +7583,7 @@
     </row>
     <row r="93" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B93">
         <v>1</v>
@@ -7657,7 +7657,7 @@
     </row>
     <row r="94" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B94">
         <v>1</v>
@@ -7731,7 +7731,7 @@
     </row>
     <row r="95" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B95">
         <v>1</v>
@@ -7805,7 +7805,7 @@
     </row>
     <row r="96" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B96">
         <v>1</v>
@@ -7879,7 +7879,7 @@
     </row>
     <row r="97" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B97">
         <v>1</v>
@@ -7953,7 +7953,7 @@
     </row>
     <row r="98" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B98">
         <v>1</v>
@@ -8027,7 +8027,7 @@
     </row>
     <row r="99" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B99">
         <v>1</v>
@@ -8101,7 +8101,7 @@
     </row>
     <row r="100" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B100">
         <v>1</v>

</xml_diff>

<commit_message>
modified decklist for tests
</commit_message>
<xml_diff>
--- a/inst/extdata/decklist.xlsx
+++ b/inst/extdata/decklist.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$X$100</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$Y$100</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
   <si>
     <t>PRODUCE UB T2</t>
   </si>
@@ -418,6 +418,9 @@
   </si>
   <si>
     <t>FarAway</t>
+  </si>
+  <si>
+    <t>enabler_ub</t>
   </si>
 </sst>
 </file>
@@ -757,23 +760,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X100"/>
+  <dimension ref="A1:Y100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A100" sqref="A100"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="12.140625" customWidth="1"/>
-    <col min="20" max="21" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>130</v>
       </c>
@@ -808,46 +811,49 @@
         <v>120</v>
       </c>
       <c r="L1" t="s">
+        <v>133</v>
+      </c>
+      <c r="M1" t="s">
         <v>100</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>121</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>122</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>103</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>102</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>101</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>124</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>125</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>126</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>127</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>128</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -894,25 +900,25 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R2">
         <v>0</v>
       </c>
       <c r="S2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W2">
         <v>0</v>
@@ -920,8 +926,11 @@
       <c r="X2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -965,10 +974,10 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -994,8 +1003,11 @@
       <c r="X3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1048,10 +1060,10 @@
         <v>0</v>
       </c>
       <c r="R4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T4">
         <v>0</v>
@@ -1060,7 +1072,7 @@
         <v>0</v>
       </c>
       <c r="V4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W4">
         <v>1</v>
@@ -1068,8 +1080,11 @@
       <c r="X4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1113,10 +1128,10 @@
         <v>0</v>
       </c>
       <c r="O5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q5">
         <v>0</v>
@@ -1142,8 +1157,11 @@
       <c r="X5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1190,10 +1208,10 @@
         <v>0</v>
       </c>
       <c r="P6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R6">
         <v>0</v>
@@ -1216,8 +1234,11 @@
       <c r="X6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1290,8 +1311,11 @@
       <c r="X7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1344,10 +1368,10 @@
         <v>0</v>
       </c>
       <c r="R8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T8">
         <v>0</v>
@@ -1356,7 +1380,7 @@
         <v>0</v>
       </c>
       <c r="V8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W8">
         <v>1</v>
@@ -1364,8 +1388,11 @@
       <c r="X8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1409,10 +1436,10 @@
         <v>0</v>
       </c>
       <c r="O9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q9">
         <v>0</v>
@@ -1438,8 +1465,11 @@
       <c r="X9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1492,10 +1522,10 @@
         <v>0</v>
       </c>
       <c r="R10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T10">
         <v>0</v>
@@ -1504,7 +1534,7 @@
         <v>0</v>
       </c>
       <c r="V10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W10">
         <v>1</v>
@@ -1512,8 +1542,11 @@
       <c r="X10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1557,10 +1590,10 @@
         <v>0</v>
       </c>
       <c r="O11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q11">
         <v>0</v>
@@ -1586,8 +1619,11 @@
       <c r="X11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>131</v>
       </c>
@@ -1631,13 +1667,13 @@
         <v>0</v>
       </c>
       <c r="O12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P12">
         <v>1</v>
       </c>
       <c r="Q12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R12">
         <v>0</v>
@@ -1660,8 +1696,11 @@
       <c r="X12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1708,10 +1747,10 @@
         <v>0</v>
       </c>
       <c r="P13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R13">
         <v>0</v>
@@ -1734,8 +1773,11 @@
       <c r="X13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1782,10 +1824,10 @@
         <v>0</v>
       </c>
       <c r="P14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R14">
         <v>0</v>
@@ -1808,8 +1850,11 @@
       <c r="X14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1856,10 +1901,10 @@
         <v>0</v>
       </c>
       <c r="P15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R15">
         <v>0</v>
@@ -1882,8 +1927,11 @@
       <c r="X15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1930,10 +1978,10 @@
         <v>0</v>
       </c>
       <c r="P16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R16">
         <v>0</v>
@@ -1956,8 +2004,11 @@
       <c r="X16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -2004,10 +2055,10 @@
         <v>0</v>
       </c>
       <c r="P17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R17">
         <v>0</v>
@@ -2030,8 +2081,11 @@
       <c r="X17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -2084,10 +2138,10 @@
         <v>0</v>
       </c>
       <c r="R18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T18">
         <v>0</v>
@@ -2096,7 +2150,7 @@
         <v>0</v>
       </c>
       <c r="V18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W18">
         <v>1</v>
@@ -2104,8 +2158,11 @@
       <c r="X18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -2152,10 +2209,10 @@
         <v>0</v>
       </c>
       <c r="P19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R19">
         <v>0</v>
@@ -2178,8 +2235,11 @@
       <c r="X19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -2223,10 +2283,10 @@
         <v>0</v>
       </c>
       <c r="O20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q20">
         <v>0</v>
@@ -2252,8 +2312,11 @@
       <c r="X20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -2300,10 +2363,10 @@
         <v>0</v>
       </c>
       <c r="P21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R21">
         <v>0</v>
@@ -2326,8 +2389,11 @@
       <c r="X21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -2374,10 +2440,10 @@
         <v>0</v>
       </c>
       <c r="P22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R22">
         <v>0</v>
@@ -2400,8 +2466,11 @@
       <c r="X22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -2445,10 +2514,10 @@
         <v>0</v>
       </c>
       <c r="O23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q23">
         <v>0</v>
@@ -2474,8 +2543,11 @@
       <c r="X23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -2519,13 +2591,13 @@
         <v>0</v>
       </c>
       <c r="O24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P24">
         <v>1</v>
       </c>
       <c r="Q24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R24">
         <v>0</v>
@@ -2548,8 +2620,11 @@
       <c r="X24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>132</v>
       </c>
@@ -2593,13 +2668,13 @@
         <v>0</v>
       </c>
       <c r="O25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P25">
         <v>1</v>
       </c>
       <c r="Q25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R25">
         <v>0</v>
@@ -2622,8 +2697,11 @@
       <c r="X25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -2667,10 +2745,10 @@
         <v>0</v>
       </c>
       <c r="O26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q26">
         <v>0</v>
@@ -2696,8 +2774,11 @@
       <c r="X26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -2750,10 +2831,10 @@
         <v>0</v>
       </c>
       <c r="R27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T27">
         <v>0</v>
@@ -2762,7 +2843,7 @@
         <v>0</v>
       </c>
       <c r="V27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W27">
         <v>1</v>
@@ -2770,8 +2851,11 @@
       <c r="X27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -2818,10 +2902,10 @@
         <v>0</v>
       </c>
       <c r="P28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R28">
         <v>0</v>
@@ -2844,8 +2928,11 @@
       <c r="X28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -2889,10 +2976,10 @@
         <v>0</v>
       </c>
       <c r="O29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q29">
         <v>0</v>
@@ -2918,8 +3005,11 @@
       <c r="X29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -2966,10 +3056,10 @@
         <v>0</v>
       </c>
       <c r="P30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R30">
         <v>0</v>
@@ -2992,8 +3082,11 @@
       <c r="X30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -3046,10 +3139,10 @@
         <v>0</v>
       </c>
       <c r="R31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T31">
         <v>0</v>
@@ -3066,8 +3159,11 @@
       <c r="X31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -3140,8 +3236,11 @@
       <c r="X32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -3188,10 +3287,10 @@
         <v>0</v>
       </c>
       <c r="P33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R33">
         <v>0</v>
@@ -3214,8 +3313,11 @@
       <c r="X33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -3259,13 +3361,13 @@
         <v>0</v>
       </c>
       <c r="O34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P34">
         <v>1</v>
       </c>
       <c r="Q34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R34">
         <v>0</v>
@@ -3288,8 +3390,11 @@
       <c r="X34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -3336,10 +3441,10 @@
         <v>0</v>
       </c>
       <c r="P35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R35">
         <v>0</v>
@@ -3362,8 +3467,11 @@
       <c r="X35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>105</v>
       </c>
@@ -3416,10 +3524,10 @@
         <v>0</v>
       </c>
       <c r="R36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T36">
         <v>0</v>
@@ -3428,16 +3536,19 @@
         <v>0</v>
       </c>
       <c r="V36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W36">
         <v>1</v>
       </c>
       <c r="X36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="Y36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>108</v>
       </c>
@@ -3490,10 +3601,10 @@
         <v>0</v>
       </c>
       <c r="R37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T37">
         <v>0</v>
@@ -3502,16 +3613,19 @@
         <v>0</v>
       </c>
       <c r="V37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W37">
         <v>1</v>
       </c>
       <c r="X37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="Y37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>109</v>
       </c>
@@ -3564,10 +3678,10 @@
         <v>0</v>
       </c>
       <c r="R38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T38">
         <v>0</v>
@@ -3576,16 +3690,19 @@
         <v>0</v>
       </c>
       <c r="V38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W38">
         <v>1</v>
       </c>
       <c r="X38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="Y38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>107</v>
       </c>
@@ -3638,10 +3755,10 @@
         <v>0</v>
       </c>
       <c r="R39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T39">
         <v>0</v>
@@ -3650,16 +3767,19 @@
         <v>0</v>
       </c>
       <c r="V39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W39">
         <v>1</v>
       </c>
       <c r="X39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="Y39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>106</v>
       </c>
@@ -3712,10 +3832,10 @@
         <v>0</v>
       </c>
       <c r="R40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T40">
         <v>0</v>
@@ -3724,16 +3844,19 @@
         <v>0</v>
       </c>
       <c r="V40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W40">
         <v>1</v>
       </c>
       <c r="X40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="Y40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>123</v>
       </c>
@@ -3786,10 +3909,10 @@
         <v>0</v>
       </c>
       <c r="R41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T41">
         <v>0</v>
@@ -3806,8 +3929,11 @@
       <c r="X41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -3854,10 +3980,10 @@
         <v>0</v>
       </c>
       <c r="P42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R42">
         <v>0</v>
@@ -3880,8 +4006,11 @@
       <c r="X42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -3954,8 +4083,11 @@
       <c r="X43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -4008,10 +4140,10 @@
         <v>0</v>
       </c>
       <c r="R44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T44">
         <v>0</v>
@@ -4020,7 +4152,7 @@
         <v>0</v>
       </c>
       <c r="V44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W44">
         <v>1</v>
@@ -4028,8 +4160,11 @@
       <c r="X44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -4102,8 +4237,11 @@
       <c r="X45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -4147,10 +4285,10 @@
         <v>0</v>
       </c>
       <c r="O46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q46">
         <v>0</v>
@@ -4176,8 +4314,11 @@
       <c r="X46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -4230,10 +4371,10 @@
         <v>0</v>
       </c>
       <c r="R47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T47">
         <v>0</v>
@@ -4242,7 +4383,7 @@
         <v>0</v>
       </c>
       <c r="V47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W47">
         <v>1</v>
@@ -4250,8 +4391,11 @@
       <c r="X47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -4324,8 +4468,11 @@
       <c r="X48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -4369,10 +4516,10 @@
         <v>0</v>
       </c>
       <c r="O49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q49">
         <v>0</v>
@@ -4398,8 +4545,11 @@
       <c r="X49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -4443,10 +4593,10 @@
         <v>0</v>
       </c>
       <c r="O50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q50">
         <v>0</v>
@@ -4472,8 +4622,11 @@
       <c r="X50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -4508,19 +4661,19 @@
         <v>0</v>
       </c>
       <c r="L51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M51">
         <v>1</v>
       </c>
       <c r="N51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q51">
         <v>0</v>
@@ -4546,8 +4699,11 @@
       <c r="X51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -4582,19 +4738,19 @@
         <v>0</v>
       </c>
       <c r="L52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M52">
         <v>1</v>
       </c>
       <c r="N52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q52">
         <v>0</v>
@@ -4620,8 +4776,11 @@
       <c r="X52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -4674,10 +4833,10 @@
         <v>0</v>
       </c>
       <c r="R53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T53">
         <v>0</v>
@@ -4686,7 +4845,7 @@
         <v>0</v>
       </c>
       <c r="V53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W53">
         <v>1</v>
@@ -4694,8 +4853,11 @@
       <c r="X53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -4739,10 +4901,10 @@
         <v>0</v>
       </c>
       <c r="O54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q54">
         <v>0</v>
@@ -4768,8 +4930,11 @@
       <c r="X54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -4822,10 +4987,10 @@
         <v>0</v>
       </c>
       <c r="R55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T55">
         <v>0</v>
@@ -4834,7 +4999,7 @@
         <v>0</v>
       </c>
       <c r="V55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W55">
         <v>1</v>
@@ -4842,8 +5007,11 @@
       <c r="X55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -4887,10 +5055,10 @@
         <v>0</v>
       </c>
       <c r="O56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q56">
         <v>0</v>
@@ -4916,8 +5084,11 @@
       <c r="X56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -4990,8 +5161,11 @@
       <c r="X57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -5064,8 +5238,11 @@
       <c r="X58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>59</v>
       </c>
@@ -5109,10 +5286,10 @@
         <v>0</v>
       </c>
       <c r="O59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q59">
         <v>0</v>
@@ -5138,8 +5315,11 @@
       <c r="X59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>60</v>
       </c>
@@ -5186,10 +5366,10 @@
         <v>0</v>
       </c>
       <c r="P60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R60">
         <v>0</v>
@@ -5212,8 +5392,11 @@
       <c r="X60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>61</v>
       </c>
@@ -5260,10 +5443,10 @@
         <v>0</v>
       </c>
       <c r="P61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R61">
         <v>0</v>
@@ -5286,8 +5469,11 @@
       <c r="X61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -5331,10 +5517,10 @@
         <v>0</v>
       </c>
       <c r="O62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q62">
         <v>0</v>
@@ -5360,8 +5546,11 @@
       <c r="X62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -5434,8 +5623,11 @@
       <c r="X63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>64</v>
       </c>
@@ -5488,10 +5680,10 @@
         <v>0</v>
       </c>
       <c r="R64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T64">
         <v>0</v>
@@ -5500,16 +5692,19 @@
         <v>0</v>
       </c>
       <c r="V64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W64">
         <v>1</v>
       </c>
       <c r="X64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="Y64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -5582,8 +5777,11 @@
       <c r="X65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -5636,10 +5834,10 @@
         <v>0</v>
       </c>
       <c r="R66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T66">
         <v>0</v>
@@ -5648,7 +5846,7 @@
         <v>0</v>
       </c>
       <c r="V66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W66">
         <v>1</v>
@@ -5656,8 +5854,11 @@
       <c r="X66">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>67</v>
       </c>
@@ -5710,10 +5911,10 @@
         <v>0</v>
       </c>
       <c r="R67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T67">
         <v>0</v>
@@ -5722,7 +5923,7 @@
         <v>0</v>
       </c>
       <c r="V67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W67">
         <v>1</v>
@@ -5730,8 +5931,11 @@
       <c r="X67">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -5766,19 +5970,19 @@
         <v>0</v>
       </c>
       <c r="L68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M68">
         <v>1</v>
       </c>
       <c r="N68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q68">
         <v>0</v>
@@ -5804,8 +6008,11 @@
       <c r="X68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>69</v>
       </c>
@@ -5849,10 +6056,10 @@
         <v>0</v>
       </c>
       <c r="O69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q69">
         <v>0</v>
@@ -5878,8 +6085,11 @@
       <c r="X69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>70</v>
       </c>
@@ -5923,10 +6133,10 @@
         <v>0</v>
       </c>
       <c r="O70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q70">
         <v>0</v>
@@ -5952,8 +6162,11 @@
       <c r="X70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>71</v>
       </c>
@@ -6006,10 +6219,10 @@
         <v>0</v>
       </c>
       <c r="R71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T71">
         <v>0</v>
@@ -6018,7 +6231,7 @@
         <v>0</v>
       </c>
       <c r="V71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W71">
         <v>1</v>
@@ -6026,8 +6239,11 @@
       <c r="X71">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>72</v>
       </c>
@@ -6071,10 +6287,10 @@
         <v>0</v>
       </c>
       <c r="O72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q72">
         <v>0</v>
@@ -6083,13 +6299,13 @@
         <v>0</v>
       </c>
       <c r="S72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T72">
         <v>1</v>
       </c>
       <c r="U72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V72">
         <v>0</v>
@@ -6100,8 +6316,11 @@
       <c r="X72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -6154,28 +6373,31 @@
         <v>0</v>
       </c>
       <c r="R73">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S73">
-        <v>0</v>
-      </c>
-      <c r="T73" s="1">
-        <v>0</v>
-      </c>
-      <c r="U73">
+        <v>1</v>
+      </c>
+      <c r="T73">
+        <v>0</v>
+      </c>
+      <c r="U73" s="1">
         <v>0</v>
       </c>
       <c r="V73">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="Y73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>74</v>
       </c>
@@ -6219,10 +6441,10 @@
         <v>0</v>
       </c>
       <c r="O74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q74">
         <v>0</v>
@@ -6248,8 +6470,11 @@
       <c r="X74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>75</v>
       </c>
@@ -6257,7 +6482,7 @@
         <v>1</v>
       </c>
       <c r="C75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -6275,7 +6500,7 @@
         <v>0</v>
       </c>
       <c r="I75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J75">
         <v>0</v>
@@ -6284,7 +6509,7 @@
         <v>0</v>
       </c>
       <c r="L75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M75">
         <v>0</v>
@@ -6293,13 +6518,13 @@
         <v>0</v>
       </c>
       <c r="O75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P75">
         <v>1</v>
       </c>
       <c r="Q75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R75">
         <v>0</v>
@@ -6322,8 +6547,11 @@
       <c r="X75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>76</v>
       </c>
@@ -6370,10 +6598,10 @@
         <v>0</v>
       </c>
       <c r="P76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R76">
         <v>0</v>
@@ -6396,8 +6624,11 @@
       <c r="X76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>77</v>
       </c>
@@ -6441,10 +6672,10 @@
         <v>0</v>
       </c>
       <c r="O77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q77">
         <v>0</v>
@@ -6470,8 +6701,11 @@
       <c r="X77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>78</v>
       </c>
@@ -6518,10 +6752,10 @@
         <v>0</v>
       </c>
       <c r="P78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R78">
         <v>0</v>
@@ -6544,8 +6778,11 @@
       <c r="X78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>79</v>
       </c>
@@ -6589,10 +6826,10 @@
         <v>0</v>
       </c>
       <c r="O79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q79">
         <v>0</v>
@@ -6618,8 +6855,11 @@
       <c r="X79">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>80</v>
       </c>
@@ -6669,10 +6909,10 @@
         <v>0</v>
       </c>
       <c r="Q80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S80">
         <v>0</v>
@@ -6692,8 +6932,11 @@
       <c r="X80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>81</v>
       </c>
@@ -6740,10 +6983,10 @@
         <v>0</v>
       </c>
       <c r="P81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R81">
         <v>0</v>
@@ -6766,8 +7009,11 @@
       <c r="X81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>82</v>
       </c>
@@ -6811,10 +7057,10 @@
         <v>0</v>
       </c>
       <c r="O82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q82">
         <v>0</v>
@@ -6840,8 +7086,11 @@
       <c r="X82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>83</v>
       </c>
@@ -6885,10 +7134,10 @@
         <v>0</v>
       </c>
       <c r="O83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q83">
         <v>0</v>
@@ -6914,8 +7163,11 @@
       <c r="X83">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>84</v>
       </c>
@@ -6968,10 +7220,10 @@
         <v>0</v>
       </c>
       <c r="R84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T84">
         <v>0</v>
@@ -6980,7 +7232,7 @@
         <v>0</v>
       </c>
       <c r="V84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W84">
         <v>1</v>
@@ -6988,8 +7240,11 @@
       <c r="X84">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>110</v>
       </c>
@@ -7042,10 +7297,10 @@
         <v>0</v>
       </c>
       <c r="R85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T85">
         <v>0</v>
@@ -7054,16 +7309,19 @@
         <v>0</v>
       </c>
       <c r="V85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="Y85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>111</v>
       </c>
@@ -7116,10 +7374,10 @@
         <v>0</v>
       </c>
       <c r="R86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T86">
         <v>0</v>
@@ -7128,16 +7386,19 @@
         <v>0</v>
       </c>
       <c r="V86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X86">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="Y86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>112</v>
       </c>
@@ -7190,10 +7451,10 @@
         <v>0</v>
       </c>
       <c r="R87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T87">
         <v>0</v>
@@ -7202,16 +7463,19 @@
         <v>0</v>
       </c>
       <c r="V87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X87">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:24" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="Y87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>113</v>
       </c>
@@ -7264,10 +7528,10 @@
         <v>0</v>
       </c>
       <c r="R88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T88">
         <v>0</v>
@@ -7276,16 +7540,19 @@
         <v>0</v>
       </c>
       <c r="V88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:24" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="Y88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>85</v>
       </c>
@@ -7329,10 +7596,10 @@
         <v>0</v>
       </c>
       <c r="O89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q89">
         <v>0</v>
@@ -7358,8 +7625,11 @@
       <c r="X89">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>86</v>
       </c>
@@ -7403,10 +7673,10 @@
         <v>0</v>
       </c>
       <c r="O90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P90">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q90">
         <v>0</v>
@@ -7432,8 +7702,11 @@
       <c r="X90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>87</v>
       </c>
@@ -7480,10 +7753,10 @@
         <v>0</v>
       </c>
       <c r="P91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R91">
         <v>0</v>
@@ -7506,8 +7779,11 @@
       <c r="X91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>88</v>
       </c>
@@ -7551,10 +7827,10 @@
         <v>0</v>
       </c>
       <c r="O92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q92">
         <v>0</v>
@@ -7580,8 +7856,11 @@
       <c r="X92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>89</v>
       </c>
@@ -7634,10 +7913,10 @@
         <v>0</v>
       </c>
       <c r="R93">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T93">
         <v>0</v>
@@ -7646,7 +7925,7 @@
         <v>0</v>
       </c>
       <c r="V93">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W93">
         <v>1</v>
@@ -7654,8 +7933,11 @@
       <c r="X93">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>90</v>
       </c>
@@ -7708,10 +7990,10 @@
         <v>0</v>
       </c>
       <c r="R94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S94">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T94">
         <v>0</v>
@@ -7720,7 +8002,7 @@
         <v>0</v>
       </c>
       <c r="V94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W94">
         <v>1</v>
@@ -7728,8 +8010,11 @@
       <c r="X94">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>91</v>
       </c>
@@ -7779,10 +8064,10 @@
         <v>0</v>
       </c>
       <c r="Q95">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S95">
         <v>0</v>
@@ -7802,8 +8087,11 @@
       <c r="X95">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>92</v>
       </c>
@@ -7850,10 +8138,10 @@
         <v>0</v>
       </c>
       <c r="P96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R96">
         <v>0</v>
@@ -7876,8 +8164,11 @@
       <c r="X96">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>93</v>
       </c>
@@ -7930,10 +8221,10 @@
         <v>0</v>
       </c>
       <c r="R97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T97">
         <v>0</v>
@@ -7942,7 +8233,7 @@
         <v>0</v>
       </c>
       <c r="V97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W97">
         <v>1</v>
@@ -7950,8 +8241,11 @@
       <c r="X97">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>94</v>
       </c>
@@ -8004,10 +8298,10 @@
         <v>0</v>
       </c>
       <c r="R98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S98">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T98">
         <v>0</v>
@@ -8016,7 +8310,7 @@
         <v>0</v>
       </c>
       <c r="V98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W98">
         <v>1</v>
@@ -8024,8 +8318,11 @@
       <c r="X98">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>95</v>
       </c>
@@ -8069,10 +8366,10 @@
         <v>0</v>
       </c>
       <c r="O99">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q99">
         <v>0</v>
@@ -8098,8 +8395,11 @@
       <c r="X99">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>96</v>
       </c>
@@ -8143,10 +8443,10 @@
         <v>0</v>
       </c>
       <c r="O100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q100">
         <v>0</v>
@@ -8172,9 +8472,12 @@
       <c r="X100">
         <v>0</v>
       </c>
+      <c r="Y100">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:X100"/>
+  <autoFilter ref="A1:Y100"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>